<commit_message>
Allow to write numeric values
</commit_message>
<xml_diff>
--- a/ExcelChef.Tests/IntegrationTests/template.xlsx
+++ b/ExcelChef.Tests/IntegrationTests/template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C306FB5-0A00-4DFD-9598-4C59DCD767E9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3B35EF-42E9-424F-ACFF-95AD09272C4B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,9 +69,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,13 +353,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -370,6 +374,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>43101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Extract utils from WriteInstruction
</commit_message>
<xml_diff>
--- a/ExcelChef.Tests/IntegrationTests/template.xlsx
+++ b/ExcelChef.Tests/IntegrationTests/template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3B35EF-42E9-424F-ACFF-95AD09272C4B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732F79B3-5757-47F5-8ECE-794E328532C2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,7 +356,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Introduce a copy instruction
</commit_message>
<xml_diff>
--- a/ExcelChef.Tests/IntegrationTests/template.xlsx
+++ b/ExcelChef.Tests/IntegrationTests/template.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732F79B3-5757-47F5-8ECE-794E328532C2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD17EB8B-98CD-4612-B752-E9A1991A00CA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEST" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -353,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -379,6 +379,12 @@
         <v>43101</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f ca="1">RAND()</f>
+        <v>8.8577696362630021E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Let the copy instruction shift formulas
</commit_message>
<xml_diff>
--- a/ExcelChef.Tests/IntegrationTests/template.xlsx
+++ b/ExcelChef.Tests/IntegrationTests/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD17EB8B-98CD-4612-B752-E9A1991A00CA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0077602F-AED1-472F-8079-98E4ACD104A9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEST" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -353,7 +353,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -382,7 +382,13 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
         <f ca="1">RAND()</f>
-        <v>8.8577696362630021E-2</v>
+        <v>0.87438849230053795</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>A1</f>
+        <v>normal</v>
       </c>
     </row>
   </sheetData>

</xml_diff>